<commit_message>
completed bootstrap module - starting bootstrap project
</commit_message>
<xml_diff>
--- a/Course Schedule.xlsx
+++ b/Course Schedule.xlsx
@@ -213,16 +213,16 @@
     <t xml:space="preserve">Section 10</t>
   </si>
   <si>
+    <t xml:space="preserve">Section 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 13</t>
   </si>
   <si>
     <t xml:space="preserve">Section 14</t>
@@ -848,15 +848,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -990,10 +990,10 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.94"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="D2" s="6" t="n">
         <f aca="false">SUM(FIN_ESTIMATES)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">SUM(DAYS_LEFT)</f>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="F2" s="7" t="n">
         <f aca="false">COUNTIF(STATUSES,"Done")/(COUNTIF(STATUSES,"Not Started")+COUNTIF(STATUSES,"In Progress")+COUNTIF(STATUSES,"Done"))</f>
-        <v>0.121621621621622</v>
+        <v>0.162162162162162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D7" s="20" t="n">
         <f aca="false">SUM(D2:D5)</f>
-        <v>32.5</v>
+        <v>38.5</v>
       </c>
       <c r="E7" s="21" t="n">
         <f aca="false">SUM(E2:E5)</f>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F7" s="22" t="n">
         <f aca="false">(D7-E7)/D7</f>
-        <v>0.369230769230769</v>
+        <v>0.467532467532468</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="D8" s="26" t="n">
         <f aca="false">SUM(D2:D6)</f>
-        <v>44.5</v>
+        <v>50.5</v>
       </c>
       <c r="E8" s="27" t="n">
         <f aca="false">SUM(E2:E6)</f>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="F8" s="28" t="n">
         <f aca="false">(D8-E8)/D8</f>
-        <v>0.269662921348315</v>
+        <v>0.356435643564356</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,15 +1219,15 @@
       </c>
       <c r="C12" s="34" t="n">
         <f aca="true">MAX(0,(B12-TODAY()+1)/7*5)</f>
-        <v>19.2857142857143</v>
+        <v>12.8571428571429</v>
       </c>
       <c r="D12" s="35" t="n">
         <f aca="true">MAX(0,(B12-NOW()+1)/7*2)</f>
-        <v>7.4537886477483</v>
+        <v>4.94198563847749</v>
       </c>
       <c r="E12" s="35" t="n">
         <f aca="false">SUM(C12:D12)</f>
-        <v>26.7395029334626</v>
+        <v>17.7991284956203</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,15 +1261,15 @@
       </c>
       <c r="B16" s="38" t="str">
         <f aca="false">ROUND(TOTAL_PLUS_EXTRA_TIME_SPENT/(DEADLINE-STARTDATE+1),1) &amp; " h/day"</f>
-        <v>0.9 h/day</v>
+        <v>1 h/day</v>
       </c>
       <c r="C16" s="38" t="str">
         <f aca="false">IF(TOTAL_DAYS_LEFT = 0, "N/A", ROUND(TOTAL_EXTRA_WORK_HOURS_LEFT/TOTAL_DAYS_LEFT,1) &amp; " h/day")</f>
-        <v>1.2 h/day</v>
+        <v>1.8 h/day</v>
       </c>
       <c r="D16" s="38" t="str">
         <f aca="true">IF(TODAY()&gt;DEADLINE, "N/A", ROUND((TOTAL_PLUS_EXTRA_TIME_SPENT-TOTAL_EXTRA_WORK_HOURS_LEFT)/(TODAY()-STARTDATE+1),1) &amp; " h/day")</f>
-        <v>0.5 h/day</v>
+        <v>0.6 h/day</v>
       </c>
       <c r="F16" s="36"/>
     </row>
@@ -1329,10 +1329,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
@@ -1379,10 +1379,7 @@
       <c r="C4" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="n">
-        <f aca="false">IF(E4 = "Done",0,C4)</f>
-        <v>0</v>
-      </c>
+      <c r="D4" s="44"/>
       <c r="E4" s="43" t="s">
         <v>32</v>
       </c>
@@ -1397,33 +1394,30 @@
       <c r="C5" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="n">
-        <f aca="false">IF(E5 = "Done",0,C5)</f>
-        <v>0</v>
-      </c>
+      <c r="D5" s="44"/>
       <c r="E5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
@@ -1435,7 +1429,7 @@
       <c r="C6" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="43" t="s">
         <v>32</v>
       </c>
@@ -1450,7 +1444,7 @@
       <c r="C7" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="43" t="s">
         <v>32</v>
       </c>
@@ -1467,7 +1461,7 @@
       <c r="C8" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="43" t="s">
         <v>32</v>
       </c>
@@ -1482,7 +1476,7 @@
       <c r="C9" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="43" t="s">
         <v>32</v>
       </c>
@@ -1497,7 +1491,7 @@
       <c r="C10" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="43" t="s">
         <v>32</v>
       </c>
@@ -1512,7 +1506,7 @@
       <c r="C11" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="43" t="s">
         <v>32</v>
       </c>
@@ -1527,7 +1521,7 @@
       <c r="C12" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="43" t="s">
         <v>32</v>
       </c>
@@ -1539,51 +1533,57 @@
       <c r="B13" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="46"/>
+      <c r="C13" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="44"/>
       <c r="E13" s="43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="46"/>
+      <c r="C14" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="44"/>
       <c r="E14" s="43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="44"/>
       <c r="E15" s="43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="43" t="n">
         <v>2</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="46"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1594,9 +1594,9 @@
         <v>2</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="46"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1607,9 +1607,9 @@
         <v>2</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="46"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1620,9 +1620,9 @@
         <v>2</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="46"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1633,9 +1633,9 @@
         <v>2</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="46"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1646,9 +1646,9 @@
         <v>2</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="46"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1659,9 +1659,9 @@
         <v>2</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="46"/>
+      <c r="D22" s="44"/>
       <c r="E22" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1672,9 +1672,9 @@
         <v>2</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="46"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1685,9 +1685,9 @@
         <v>2</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="46"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1698,9 +1698,9 @@
         <v>2</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="46"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1711,9 +1711,9 @@
         <v>2</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="46"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1724,9 +1724,9 @@
         <v>2</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="46"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1737,9 +1737,9 @@
         <v>2</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="46"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1750,9 +1750,9 @@
         <v>2</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="46"/>
+      <c r="D29" s="44"/>
       <c r="E29" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1763,9 +1763,9 @@
         <v>2</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="46"/>
+      <c r="D30" s="44"/>
       <c r="E30" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1775,9 +1775,9 @@
       <c r="B31" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D31" s="46"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1788,9 +1788,9 @@
         <v>2</v>
       </c>
       <c r="C32" s="10"/>
-      <c r="D32" s="46"/>
+      <c r="D32" s="44"/>
       <c r="E32" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1801,9 +1801,9 @@
         <v>2</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="46"/>
+      <c r="D33" s="44"/>
       <c r="E33" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +1847,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1902,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +1924,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,7 +1957,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,7 +1979,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2001,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2012,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,7 +2023,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2056,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,7 +2067,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="E58" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,7 +2122,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2144,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,7 +2155,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,7 +2199,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,7 +2210,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,7 +2221,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="E74" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2265,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2353,7 @@
       <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -2398,12 +2398,12 @@
       <c r="C4" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="44" t="n">
         <f aca="false">IF(E4 = "Done",0,C4)</f>
         <v>1</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,33 +2416,33 @@
       <c r="C5" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="44" t="n">
         <f aca="false">IF(E5 = "Done",0,C5)</f>
         <v>1</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
@@ -2454,33 +2454,33 @@
       <c r="C6" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="44" t="n">
         <f aca="false">IF(E6 = "Done",0,C6)</f>
         <v>1</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
@@ -2492,33 +2492,33 @@
       <c r="C7" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="44" t="n">
         <f aca="false">IF(E7 = "Done",0,C7)</f>
         <v>1</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="43" t="s">
@@ -2530,33 +2530,33 @@
       <c r="C8" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="44" t="n">
         <f aca="false">IF(E8 = "Done",0,C8)</f>
         <v>1</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="43" t="s">
@@ -2568,33 +2568,33 @@
       <c r="C9" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="46" t="n">
+      <c r="D9" s="44" t="n">
         <f aca="false">IF(E9 = "Done",0,C9)</f>
         <v>1</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
@@ -2606,33 +2606,33 @@
       <c r="C10" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="46" t="n">
+      <c r="D10" s="44" t="n">
         <f aca="false">IF(E10 = "Done",0,C10)</f>
         <v>1</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="45"/>
-      <c r="W10" s="45"/>
-      <c r="X10" s="45"/>
-      <c r="Y10" s="45"/>
-      <c r="Z10" s="45"/>
-      <c r="AA10" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30"/>
@@ -2765,7 +2765,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -2810,12 +2810,12 @@
       <c r="C4" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="44" t="n">
         <f aca="false">IF(E4 = "Done",0,C4)</f>
         <v>0.5</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,33 +2828,33 @@
       <c r="C5" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="44" t="n">
         <f aca="false">IF(E5 = "Done",0,C5)</f>
         <v>0.5</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
@@ -2866,33 +2866,33 @@
       <c r="C6" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="44" t="n">
         <f aca="false">IF(E6 = "Done",0,C6)</f>
         <v>0.5</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
@@ -2904,33 +2904,33 @@
       <c r="C7" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="44" t="n">
         <f aca="false">IF(E7 = "Done",0,C7)</f>
         <v>0.5</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="43" t="s">
@@ -2942,33 +2942,33 @@
       <c r="C8" s="43" t="n">
         <v>0.5</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="44" t="n">
         <f aca="false">IF(E8 = "Done",0,C8)</f>
         <v>0.5</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="43" t="s">
@@ -2980,33 +2980,33 @@
       <c r="C9" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="46" t="n">
+      <c r="D9" s="44" t="n">
         <f aca="false">IF(E9 = "Done",0,C9)</f>
         <v>1</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
@@ -3018,33 +3018,33 @@
       <c r="C10" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="46" t="n">
+      <c r="D10" s="44" t="n">
         <f aca="false">IF(E10 = "Done",0,C10)</f>
         <v>1</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="45"/>
-      <c r="W10" s="45"/>
-      <c r="X10" s="45"/>
-      <c r="Y10" s="45"/>
-      <c r="Z10" s="45"/>
-      <c r="AA10" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+      <c r="AA10" s="46"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="48"/>
@@ -3164,7 +3164,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -3209,12 +3209,12 @@
       <c r="C4" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="44" t="n">
         <f aca="false">IF(E4 = "Done",0,C4)</f>
         <v>3</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,33 +3227,33 @@
       <c r="C5" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="44" t="n">
         <f aca="false">IF(E5 = "Done",0,C5)</f>
         <v>3</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
@@ -3265,12 +3265,12 @@
       <c r="C6" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="44" t="n">
         <f aca="false">IF(E6 = "Done",0,C6)</f>
         <v>3</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3357,7 @@
       <selection pane="bottomLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -3402,12 +3402,12 @@
       <c r="C4" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="44" t="n">
         <f aca="false">IF(E4 = "Done",0,C4)</f>
         <v>2</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,33 +3420,33 @@
       <c r="C5" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="44" t="n">
         <f aca="false">IF(E5 = "Done",0,C5)</f>
         <v>2</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
@@ -3458,33 +3458,33 @@
       <c r="C6" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="44" t="n">
         <f aca="false">IF(E6 = "Done",0,C6)</f>
         <v>2</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
@@ -3496,33 +3496,33 @@
       <c r="C7" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="44" t="n">
         <f aca="false">IF(E7 = "Done",0,C7)</f>
         <v>2</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="43" t="s">
@@ -3534,33 +3534,33 @@
       <c r="C8" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="44" t="n">
         <f aca="false">IF(E8 = "Done",0,C8)</f>
         <v>2</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+      <c r="AA8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="43" t="s">
@@ -3572,33 +3572,33 @@
       <c r="C9" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="46" t="n">
+      <c r="D9" s="44" t="n">
         <f aca="false">IF(E9 = "Done",0,C9)</f>
         <v>2</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="30"/>
@@ -3714,7 +3714,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.25"/>
   </cols>

</xml_diff>